<commit_message>
Add FontScheme to an IXLFontbase. FontScheme is an attribute of a CT_Font element in style part, so it can be used in cells and all other places that reference main font table. The original implementation used it only for rich text that saves font scheme along with other font properties to a separate place (rich text run).
Thanks to improved font equality check, the CanLoadFromTemplate now fails (one font is now different and thus there are two), but fix requires addition of namespace + ignorable to 100+ files,so in subsequent commit.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Styles/StyleFont.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Styles/StyleFont.xlsx
@@ -45,6 +45,9 @@
   <x:si>
     <x:t>VerticalAlignment - Superscript</x:t>
   </x:si>
+  <x:si>
+    <x:t>FontScheme - Major</x:t>
+  </x:si>
 </x:sst>
 </file>
 
@@ -53,7 +56,7 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="11">
+  <x:fonts count="12">
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
@@ -135,6 +138,14 @@
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
       <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="major"/>
     </x:font>
   </x:fonts>
   <x:fills count="2">
@@ -164,7 +175,7 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="11">
+  <x:cellStyleXfs count="12">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -198,8 +209,11 @@
     <x:xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="11">
+  <x:cellXfs count="12">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -241,6 +255,10 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -539,7 +557,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B11"/>
+  <x:dimension ref="A1:B12"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -599,6 +617,11 @@
         <x:v>9</x:v>
       </x:c>
     </x:row>
+    <x:row r="12" spans="1:2">
+      <x:c r="B12" s="11" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>